<commit_message>
added rest of archive data to tables
</commit_message>
<xml_diff>
--- a/A004/table1.xlsx
+++ b/A004/table1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\Desktop\Universitaet\Fortgeschrittenes_Praktikum_I\advanced_labcourse\A004\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Lukas_Prader\uibk\Physik_Unterlagen\6.Semester\Fortgeschrittenenpraktikum_1\advanced_labcourse\A004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37881F9-B579-4971-89E2-4807C2BE7EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E74E8F2-BFE1-4453-99C8-30415295E7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6223" yWindow="5511" windowWidth="15377" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="15">
   <si>
     <t>iteration</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>ir</t>
+  </si>
+  <si>
+    <t>w</t>
   </si>
 </sst>
 </file>
@@ -603,17 +606,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="J150" sqref="J150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="4" width="10.640625" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="8" width="10.640625" customWidth="1"/>
+    <col min="1" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3656,6 +3659,1150 @@
       </c>
       <c r="H117" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>2022</v>
+      </c>
+      <c r="E118" s="1">
+        <v>9625.3459999999995</v>
+      </c>
+      <c r="F118" s="1">
+        <v>102.515</v>
+      </c>
+      <c r="G118">
+        <v>57.388820000000003</v>
+      </c>
+      <c r="H118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
+      <c r="A119" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119">
+        <v>10</v>
+      </c>
+      <c r="D119">
+        <v>2022</v>
+      </c>
+      <c r="E119" s="1">
+        <v>11037.47</v>
+      </c>
+      <c r="F119" s="1">
+        <v>92.282849999999996</v>
+      </c>
+      <c r="G119">
+        <v>51.98151</v>
+      </c>
+      <c r="H119" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
+      <c r="A120" t="s">
+        <v>8</v>
+      </c>
+      <c r="B120" t="s">
+        <v>14</v>
+      </c>
+      <c r="C120">
+        <v>20</v>
+      </c>
+      <c r="D120">
+        <v>2022</v>
+      </c>
+      <c r="E120" s="1">
+        <v>12733.64</v>
+      </c>
+      <c r="F120" s="1">
+        <v>123.8691</v>
+      </c>
+      <c r="G120">
+        <v>47.645200000000003</v>
+      </c>
+      <c r="H120" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
+      <c r="A121" t="s">
+        <v>8</v>
+      </c>
+      <c r="B121" t="s">
+        <v>14</v>
+      </c>
+      <c r="C121">
+        <v>30</v>
+      </c>
+      <c r="D121">
+        <v>2022</v>
+      </c>
+      <c r="E121" s="1">
+        <v>14773.96</v>
+      </c>
+      <c r="F121" s="1">
+        <v>97.925129999999996</v>
+      </c>
+      <c r="G121">
+        <v>44.717939999999999</v>
+      </c>
+      <c r="H121" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
+      <c r="A122" t="s">
+        <v>8</v>
+      </c>
+      <c r="B122" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122">
+        <v>40</v>
+      </c>
+      <c r="D122">
+        <v>2022</v>
+      </c>
+      <c r="E122" s="1">
+        <v>17733.12</v>
+      </c>
+      <c r="F122" s="1">
+        <v>17925.66</v>
+      </c>
+      <c r="G122">
+        <v>43.49738</v>
+      </c>
+      <c r="H122" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
+      <c r="A123" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123">
+        <v>50</v>
+      </c>
+      <c r="D123">
+        <v>2022</v>
+      </c>
+      <c r="E123" s="1">
+        <v>20771.62</v>
+      </c>
+      <c r="F123" s="1">
+        <v>202.8767</v>
+      </c>
+      <c r="G123">
+        <v>44.143219999999999</v>
+      </c>
+      <c r="H123" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
+      <c r="A124" t="s">
+        <v>8</v>
+      </c>
+      <c r="B124" t="s">
+        <v>14</v>
+      </c>
+      <c r="C124">
+        <v>60</v>
+      </c>
+      <c r="D124">
+        <v>2022</v>
+      </c>
+      <c r="E124" s="1">
+        <v>25926.71</v>
+      </c>
+      <c r="F124" s="1">
+        <v>169.88149999999999</v>
+      </c>
+      <c r="G124">
+        <v>46.557369999999999</v>
+      </c>
+      <c r="H124" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
+      <c r="A125" t="s">
+        <v>8</v>
+      </c>
+      <c r="B125" t="s">
+        <v>14</v>
+      </c>
+      <c r="C125">
+        <v>65</v>
+      </c>
+      <c r="D125">
+        <v>2022</v>
+      </c>
+      <c r="E125" s="1">
+        <v>29282.06</v>
+      </c>
+      <c r="F125" s="1">
+        <v>261.7724</v>
+      </c>
+      <c r="G125">
+        <v>48.392159999999997</v>
+      </c>
+      <c r="H125" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
+      <c r="A126" t="s">
+        <v>8</v>
+      </c>
+      <c r="B126" t="s">
+        <v>14</v>
+      </c>
+      <c r="C126">
+        <v>70</v>
+      </c>
+      <c r="D126">
+        <v>2022</v>
+      </c>
+      <c r="E126" s="1">
+        <v>35166.639999999999</v>
+      </c>
+      <c r="F126" s="1">
+        <v>319.96949999999998</v>
+      </c>
+      <c r="G126">
+        <v>50.562199999999997</v>
+      </c>
+      <c r="H126" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
+      <c r="A127" t="s">
+        <v>8</v>
+      </c>
+      <c r="B127" t="s">
+        <v>14</v>
+      </c>
+      <c r="C127">
+        <v>75</v>
+      </c>
+      <c r="D127">
+        <v>2022</v>
+      </c>
+      <c r="E127" s="1">
+        <v>42994.41</v>
+      </c>
+      <c r="F127" s="1">
+        <v>439.06079999999997</v>
+      </c>
+      <c r="G127">
+        <v>53.033769999999997</v>
+      </c>
+      <c r="H127" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
+      <c r="A128" t="s">
+        <v>8</v>
+      </c>
+      <c r="B128" t="s">
+        <v>14</v>
+      </c>
+      <c r="C128">
+        <v>80</v>
+      </c>
+      <c r="D128">
+        <v>2022</v>
+      </c>
+      <c r="E128" s="1">
+        <v>56513.95</v>
+      </c>
+      <c r="F128" s="1">
+        <v>571.9769</v>
+      </c>
+      <c r="G128">
+        <v>55.772680000000001</v>
+      </c>
+      <c r="H128" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
+      <c r="A129" t="s">
+        <v>8</v>
+      </c>
+      <c r="B129" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>2022</v>
+      </c>
+      <c r="E129" s="1">
+        <v>28173.45</v>
+      </c>
+      <c r="F129" s="1">
+        <v>29351.42</v>
+      </c>
+      <c r="G129">
+        <v>57.388820000000003</v>
+      </c>
+      <c r="H129" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
+      <c r="A130" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" t="s">
+        <v>14</v>
+      </c>
+      <c r="C130">
+        <v>10</v>
+      </c>
+      <c r="D130">
+        <v>2022</v>
+      </c>
+      <c r="E130" s="1">
+        <v>31493.29</v>
+      </c>
+      <c r="F130" s="1">
+        <v>837.00739999999996</v>
+      </c>
+      <c r="G130">
+        <v>51.98151</v>
+      </c>
+      <c r="H130" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
+      <c r="A131" t="s">
+        <v>8</v>
+      </c>
+      <c r="B131" t="s">
+        <v>14</v>
+      </c>
+      <c r="C131">
+        <v>20</v>
+      </c>
+      <c r="D131">
+        <v>2022</v>
+      </c>
+      <c r="E131" s="1">
+        <v>35464.43</v>
+      </c>
+      <c r="F131" s="1">
+        <v>955.76260000000002</v>
+      </c>
+      <c r="G131">
+        <v>47.645200000000003</v>
+      </c>
+      <c r="H131" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
+      <c r="A132" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" t="s">
+        <v>14</v>
+      </c>
+      <c r="C132">
+        <v>30</v>
+      </c>
+      <c r="D132">
+        <v>2022</v>
+      </c>
+      <c r="E132" s="1">
+        <v>40512.89</v>
+      </c>
+      <c r="F132" s="1">
+        <v>1084.0609999999999</v>
+      </c>
+      <c r="G132">
+        <v>44.717939999999999</v>
+      </c>
+      <c r="H132" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
+      <c r="A133" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" t="s">
+        <v>14</v>
+      </c>
+      <c r="C133">
+        <v>40</v>
+      </c>
+      <c r="D133">
+        <v>2022</v>
+      </c>
+      <c r="E133" s="1">
+        <v>47265.64</v>
+      </c>
+      <c r="F133" s="1">
+        <v>1292.8789999999999</v>
+      </c>
+      <c r="G133">
+        <v>43.49738</v>
+      </c>
+      <c r="H133" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
+      <c r="A134" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" t="s">
+        <v>14</v>
+      </c>
+      <c r="C134">
+        <v>50</v>
+      </c>
+      <c r="D134">
+        <v>2022</v>
+      </c>
+      <c r="E134" s="1">
+        <v>53831.49</v>
+      </c>
+      <c r="F134" s="1">
+        <v>1496.278</v>
+      </c>
+      <c r="G134">
+        <v>44.143219999999999</v>
+      </c>
+      <c r="H134" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
+      <c r="A135" t="s">
+        <v>8</v>
+      </c>
+      <c r="B135" t="s">
+        <v>14</v>
+      </c>
+      <c r="C135">
+        <v>60</v>
+      </c>
+      <c r="D135">
+        <v>2022</v>
+      </c>
+      <c r="E135" s="1">
+        <v>64169.279999999999</v>
+      </c>
+      <c r="F135" s="1">
+        <v>1775.31</v>
+      </c>
+      <c r="G135">
+        <v>46.557369999999999</v>
+      </c>
+      <c r="H135" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" t="s">
+        <v>8</v>
+      </c>
+      <c r="B136" t="s">
+        <v>14</v>
+      </c>
+      <c r="C136">
+        <v>65</v>
+      </c>
+      <c r="D136">
+        <v>2022</v>
+      </c>
+      <c r="E136" s="1">
+        <v>70508.899999999994</v>
+      </c>
+      <c r="F136" s="1">
+        <v>1886.0730000000001</v>
+      </c>
+      <c r="G136">
+        <v>48.392159999999997</v>
+      </c>
+      <c r="H136" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
+      <c r="A137" t="s">
+        <v>8</v>
+      </c>
+      <c r="B137" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137">
+        <v>70</v>
+      </c>
+      <c r="D137">
+        <v>2022</v>
+      </c>
+      <c r="E137" s="1">
+        <v>80602.490000000005</v>
+      </c>
+      <c r="F137" s="1">
+        <v>2155.1799999999998</v>
+      </c>
+      <c r="G137">
+        <v>50.562199999999997</v>
+      </c>
+      <c r="H137" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138" t="s">
+        <v>14</v>
+      </c>
+      <c r="C138">
+        <v>75</v>
+      </c>
+      <c r="D138">
+        <v>2022</v>
+      </c>
+      <c r="E138" s="1">
+        <v>90430.77</v>
+      </c>
+      <c r="F138" s="1">
+        <v>2495.5410000000002</v>
+      </c>
+      <c r="G138">
+        <v>53.033769999999997</v>
+      </c>
+      <c r="H138" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" t="s">
+        <v>8</v>
+      </c>
+      <c r="B139" t="s">
+        <v>14</v>
+      </c>
+      <c r="C139">
+        <v>80</v>
+      </c>
+      <c r="D139">
+        <v>2022</v>
+      </c>
+      <c r="E139" s="1">
+        <v>100414.5</v>
+      </c>
+      <c r="F139" s="1">
+        <v>2876.1689999999999</v>
+      </c>
+      <c r="G139">
+        <v>55.772680000000001</v>
+      </c>
+      <c r="H139" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" t="s">
+        <v>8</v>
+      </c>
+      <c r="B140" t="s">
+        <v>14</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>2022</v>
+      </c>
+      <c r="E140" s="1">
+        <v>21217.02</v>
+      </c>
+      <c r="F140" s="1">
+        <v>353.55029999999999</v>
+      </c>
+      <c r="G140">
+        <v>57.388820000000003</v>
+      </c>
+      <c r="H140" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" t="s">
+        <v>8</v>
+      </c>
+      <c r="B141" t="s">
+        <v>14</v>
+      </c>
+      <c r="C141">
+        <v>10</v>
+      </c>
+      <c r="D141">
+        <v>2022</v>
+      </c>
+      <c r="E141" s="1">
+        <v>24154.75</v>
+      </c>
+      <c r="F141" s="1">
+        <v>384.37450000000001</v>
+      </c>
+      <c r="G141">
+        <v>51.98151</v>
+      </c>
+      <c r="H141" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142" t="s">
+        <v>14</v>
+      </c>
+      <c r="C142">
+        <v>20</v>
+      </c>
+      <c r="D142">
+        <v>2022</v>
+      </c>
+      <c r="E142" s="1">
+        <v>27816.28</v>
+      </c>
+      <c r="F142" s="1">
+        <v>528.97810000000004</v>
+      </c>
+      <c r="G142">
+        <v>47.645200000000003</v>
+      </c>
+      <c r="H142" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" t="s">
+        <v>8</v>
+      </c>
+      <c r="B143" t="s">
+        <v>14</v>
+      </c>
+      <c r="C143">
+        <v>30</v>
+      </c>
+      <c r="D143">
+        <v>2022</v>
+      </c>
+      <c r="E143" s="1">
+        <v>32204.41</v>
+      </c>
+      <c r="F143" s="1">
+        <v>584.53930000000003</v>
+      </c>
+      <c r="G143">
+        <v>44.717939999999999</v>
+      </c>
+      <c r="H143" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" t="s">
+        <v>14</v>
+      </c>
+      <c r="C144">
+        <v>40</v>
+      </c>
+      <c r="D144">
+        <v>2022</v>
+      </c>
+      <c r="E144" s="1">
+        <v>38047.85</v>
+      </c>
+      <c r="F144" s="1">
+        <v>697.75189999999998</v>
+      </c>
+      <c r="G144">
+        <v>43.49738</v>
+      </c>
+      <c r="H144" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="A145" t="s">
+        <v>8</v>
+      </c>
+      <c r="B145" t="s">
+        <v>14</v>
+      </c>
+      <c r="C145">
+        <v>50</v>
+      </c>
+      <c r="D145">
+        <v>2022</v>
+      </c>
+      <c r="E145" s="1">
+        <v>43905.34</v>
+      </c>
+      <c r="F145" s="1">
+        <v>825.19399999999996</v>
+      </c>
+      <c r="G145">
+        <v>44.143219999999999</v>
+      </c>
+      <c r="H145" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146" t="s">
+        <v>14</v>
+      </c>
+      <c r="C146">
+        <v>60</v>
+      </c>
+      <c r="D146">
+        <v>2022</v>
+      </c>
+      <c r="E146" s="1">
+        <v>53457.55</v>
+      </c>
+      <c r="F146" s="1">
+        <v>1009.614</v>
+      </c>
+      <c r="G146">
+        <v>46.557369999999999</v>
+      </c>
+      <c r="H146" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147" t="s">
+        <v>14</v>
+      </c>
+      <c r="C147">
+        <v>65</v>
+      </c>
+      <c r="D147">
+        <v>2022</v>
+      </c>
+      <c r="E147" s="1">
+        <v>59368.12</v>
+      </c>
+      <c r="F147" s="1">
+        <v>1227.04</v>
+      </c>
+      <c r="G147">
+        <v>48.392159999999997</v>
+      </c>
+      <c r="H147" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" t="s">
+        <v>14</v>
+      </c>
+      <c r="C148">
+        <v>70</v>
+      </c>
+      <c r="D148">
+        <v>2022</v>
+      </c>
+      <c r="E148" s="1">
+        <v>69157.69</v>
+      </c>
+      <c r="F148" s="1">
+        <v>1477.0740000000001</v>
+      </c>
+      <c r="G148">
+        <v>50.562199999999997</v>
+      </c>
+      <c r="H148" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" t="s">
+        <v>14</v>
+      </c>
+      <c r="C149">
+        <v>75</v>
+      </c>
+      <c r="D149">
+        <v>2022</v>
+      </c>
+      <c r="E149" s="1">
+        <v>81140.42</v>
+      </c>
+      <c r="F149" s="1">
+        <v>1875.8510000000001</v>
+      </c>
+      <c r="G149">
+        <v>53.033769999999997</v>
+      </c>
+      <c r="H149" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150" t="s">
+        <v>14</v>
+      </c>
+      <c r="C150">
+        <v>80</v>
+      </c>
+      <c r="D150">
+        <v>2022</v>
+      </c>
+      <c r="E150" s="1">
+        <v>98582.32</v>
+      </c>
+      <c r="F150" s="1">
+        <v>2727.3870000000002</v>
+      </c>
+      <c r="G150">
+        <v>55.772680000000001</v>
+      </c>
+      <c r="H150" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" t="s">
+        <v>14</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>2022</v>
+      </c>
+      <c r="E151" s="1">
+        <v>10893.52</v>
+      </c>
+      <c r="F151" s="1">
+        <v>97.48518</v>
+      </c>
+      <c r="G151">
+        <v>57.388820000000003</v>
+      </c>
+      <c r="H151" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152" t="s">
+        <v>8</v>
+      </c>
+      <c r="B152" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152">
+        <v>10</v>
+      </c>
+      <c r="D152">
+        <v>2022</v>
+      </c>
+      <c r="E152" s="1">
+        <v>12451.1</v>
+      </c>
+      <c r="F152" s="1">
+        <v>85.148929999999993</v>
+      </c>
+      <c r="G152">
+        <v>51.98151</v>
+      </c>
+      <c r="H152" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="A153" t="s">
+        <v>8</v>
+      </c>
+      <c r="B153" t="s">
+        <v>14</v>
+      </c>
+      <c r="C153">
+        <v>20</v>
+      </c>
+      <c r="D153">
+        <v>2022</v>
+      </c>
+      <c r="E153" s="1">
+        <v>14412.85</v>
+      </c>
+      <c r="F153" s="1">
+        <v>121.5947</v>
+      </c>
+      <c r="G153">
+        <v>47.645200000000003</v>
+      </c>
+      <c r="H153" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="A154" t="s">
+        <v>8</v>
+      </c>
+      <c r="B154" t="s">
+        <v>14</v>
+      </c>
+      <c r="C154">
+        <v>30</v>
+      </c>
+      <c r="D154">
+        <v>2022</v>
+      </c>
+      <c r="E154" s="1">
+        <v>16714.16</v>
+      </c>
+      <c r="F154" s="1">
+        <v>135.93530000000001</v>
+      </c>
+      <c r="G154">
+        <v>44.717939999999999</v>
+      </c>
+      <c r="H154" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="A155" t="s">
+        <v>8</v>
+      </c>
+      <c r="B155" t="s">
+        <v>14</v>
+      </c>
+      <c r="C155">
+        <v>40</v>
+      </c>
+      <c r="D155">
+        <v>2022</v>
+      </c>
+      <c r="E155" s="1">
+        <v>19975.13</v>
+      </c>
+      <c r="F155" s="1">
+        <v>144.47470000000001</v>
+      </c>
+      <c r="G155">
+        <v>43.49738</v>
+      </c>
+      <c r="H155" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="A156" t="s">
+        <v>8</v>
+      </c>
+      <c r="B156" t="s">
+        <v>14</v>
+      </c>
+      <c r="C156">
+        <v>50</v>
+      </c>
+      <c r="D156">
+        <v>2022</v>
+      </c>
+      <c r="E156" s="1">
+        <v>23192.43</v>
+      </c>
+      <c r="F156" s="1">
+        <v>126.2409</v>
+      </c>
+      <c r="G156">
+        <v>44.143219999999999</v>
+      </c>
+      <c r="H156" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="A157" t="s">
+        <v>8</v>
+      </c>
+      <c r="B157" t="s">
+        <v>14</v>
+      </c>
+      <c r="C157">
+        <v>60</v>
+      </c>
+      <c r="D157">
+        <v>2022</v>
+      </c>
+      <c r="E157" s="1">
+        <v>28605.81</v>
+      </c>
+      <c r="F157" s="1">
+        <v>187.32310000000001</v>
+      </c>
+      <c r="G157">
+        <v>46.557369999999999</v>
+      </c>
+      <c r="H157" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158" t="s">
+        <v>8</v>
+      </c>
+      <c r="B158" t="s">
+        <v>14</v>
+      </c>
+      <c r="C158">
+        <v>65</v>
+      </c>
+      <c r="D158">
+        <v>2022</v>
+      </c>
+      <c r="E158" s="1">
+        <v>32011.09</v>
+      </c>
+      <c r="F158" s="1">
+        <v>199.78210000000001</v>
+      </c>
+      <c r="G158">
+        <v>48.392159999999997</v>
+      </c>
+      <c r="H158" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="A159" t="s">
+        <v>8</v>
+      </c>
+      <c r="B159" t="s">
+        <v>14</v>
+      </c>
+      <c r="C159">
+        <v>70</v>
+      </c>
+      <c r="D159">
+        <v>2022</v>
+      </c>
+      <c r="E159" s="1">
+        <v>37863.449999999997</v>
+      </c>
+      <c r="F159" s="1">
+        <v>245.86330000000001</v>
+      </c>
+      <c r="G159">
+        <v>50.562199999999997</v>
+      </c>
+      <c r="H159" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="A160" t="s">
+        <v>8</v>
+      </c>
+      <c r="B160" t="s">
+        <v>14</v>
+      </c>
+      <c r="C160">
+        <v>75</v>
+      </c>
+      <c r="D160">
+        <v>2022</v>
+      </c>
+      <c r="E160" s="1">
+        <v>45398.89</v>
+      </c>
+      <c r="F160" s="1">
+        <v>288.358</v>
+      </c>
+      <c r="G160">
+        <v>53.033769999999997</v>
+      </c>
+      <c r="H160" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="A161" t="s">
+        <v>8</v>
+      </c>
+      <c r="B161" t="s">
+        <v>14</v>
+      </c>
+      <c r="C161">
+        <v>80</v>
+      </c>
+      <c r="D161">
+        <v>2022</v>
+      </c>
+      <c r="E161" s="1">
+        <v>57490.55</v>
+      </c>
+      <c r="F161" s="1">
+        <v>398.66030000000001</v>
+      </c>
+      <c r="G161">
+        <v>55.772680000000001</v>
+      </c>
+      <c r="H161" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new approach to intensity fit + data correction
</commit_message>
<xml_diff>
--- a/A004/table1.xlsx
+++ b/A004/table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Documents\Lukas_Prader\uibk\Physik_Unterlagen\6.Semester\Fortgeschrittenenpraktikum_1\advanced_labcourse\A004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E74E8F2-BFE1-4453-99C8-30415295E7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533456F3-2B5A-41D3-B318-8A03BA8C389A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="J150" sqref="J150"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3782,7 +3782,7 @@
         <v>17733.12</v>
       </c>
       <c r="F122" s="1">
-        <v>17925.66</v>
+        <v>154.32740000000001</v>
       </c>
       <c r="G122">
         <v>43.49738</v>
@@ -3964,7 +3964,7 @@
         <v>28173.45</v>
       </c>
       <c r="F129" s="1">
-        <v>29351.42</v>
+        <v>771.78250000000003</v>
       </c>
       <c r="G129">
         <v>57.388820000000003</v>

</xml_diff>